<commit_message>
manaual discount test data update and keywords
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Promo/promo_test_data.xlsx
+++ b/TestData/Web_POS/Promo/promo_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anand\PycharmProjects\Zwing QA Automation\zwing-qa-automation\TestData\POS\Promo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Ginesys Zwing\Ginesys_Zwing_Automation\TestData\POS\Promo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -90,13 +90,13 @@
     <t>TC_01</t>
   </si>
   <si>
-    <t>307220324rGH</t>
+    <t>307220324WWP</t>
   </si>
   <si>
     <t>zwshashank.agrawal@teampureplay.com</t>
   </si>
   <si>
-    <t>AnandArya</t>
+    <t>i9Qa_user1</t>
   </si>
   <si>
     <t>Index9QA</t>
@@ -579,25 +579,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
-    <border>
-      <left>
-        <color indexed="64"/>
-      </left>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-      <diagonal>
-        <color indexed="64"/>
-      </diagonal>
-    </border>
     <border>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -610,16 +593,15 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -847,8 +829,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A44">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="F1">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -954,7 +936,7 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -978,7 +960,7 @@
       <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="1">
@@ -993,13 +975,13 @@
       <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="5" t="s">
+      <c r="O2" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -1022,7 +1004,7 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1046,7 +1028,7 @@
       <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="K3" s="1">
@@ -1061,13 +1043,13 @@
       <c r="N3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="O3" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -1090,7 +1072,7 @@
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1114,7 +1096,7 @@
       <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="K4" s="1">
@@ -1129,13 +1111,13 @@
       <c r="N4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="O4" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1158,7 +1140,7 @@
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1182,7 +1164,7 @@
       <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="1">
@@ -1197,13 +1179,13 @@
       <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="5" t="s">
+      <c r="O5" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -1226,7 +1208,7 @@
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1250,7 +1232,7 @@
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="K6" s="1">
@@ -1265,13 +1247,13 @@
       <c r="N6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="5" t="s">
+      <c r="O6" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1294,7 +1276,7 @@
       <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1318,7 +1300,7 @@
       <c r="I7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="K7" s="1">
@@ -1333,13 +1315,13 @@
       <c r="N7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="5" t="s">
+      <c r="O7" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -1362,7 +1344,7 @@
       <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1386,7 +1368,7 @@
       <c r="I8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>48</v>
       </c>
       <c r="K8" s="1">
@@ -1401,13 +1383,13 @@
       <c r="N8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="5" t="s">
+      <c r="O8" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -1430,7 +1412,7 @@
       <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1454,7 +1436,7 @@
       <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="1">
@@ -1469,13 +1451,13 @@
       <c r="N9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q9" s="5" t="s">
+      <c r="O9" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -1498,7 +1480,7 @@
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1522,7 +1504,7 @@
       <c r="I10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="K10" s="1">
@@ -1537,13 +1519,13 @@
       <c r="N10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="5" t="s">
+      <c r="O10" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1566,7 +1548,7 @@
       <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1590,7 +1572,7 @@
       <c r="I11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>56</v>
       </c>
       <c r="K11" s="1">
@@ -1605,13 +1587,13 @@
       <c r="N11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q11" s="5" t="s">
+      <c r="O11" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -1634,7 +1616,7 @@
       <c r="A12" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1658,7 +1640,7 @@
       <c r="I12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>59</v>
       </c>
       <c r="K12" s="1">
@@ -1673,13 +1655,13 @@
       <c r="N12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q12" s="5" t="s">
+      <c r="O12" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -1702,7 +1684,7 @@
       <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1741,13 +1723,13 @@
       <c r="N13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q13" s="5" t="s">
+      <c r="O13" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1770,7 +1752,7 @@
       <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1809,13 +1791,13 @@
       <c r="N14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q14" s="5" t="s">
+      <c r="O14" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -1838,7 +1820,7 @@
       <c r="A15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1877,13 +1859,13 @@
       <c r="N15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q15" s="5" t="s">
+      <c r="O15" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R15" s="1" t="s">
@@ -1906,7 +1888,7 @@
       <c r="A16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1945,13 +1927,13 @@
       <c r="N16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O16" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q16" s="5" t="s">
+      <c r="O16" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1974,7 +1956,7 @@
       <c r="A17" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2013,13 +1995,13 @@
       <c r="N17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q17" s="5" t="s">
+      <c r="O17" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R17" s="1" t="s">
@@ -2042,7 +2024,7 @@
       <c r="A18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2081,13 +2063,13 @@
       <c r="N18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O18" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q18" s="5" t="s">
+      <c r="O18" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -2110,7 +2092,7 @@
       <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2149,13 +2131,13 @@
       <c r="N19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O19" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q19" s="5" t="s">
+      <c r="O19" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R19" s="1" t="s">
@@ -2178,7 +2160,7 @@
       <c r="A20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -2217,13 +2199,13 @@
       <c r="N20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q20" s="5" t="s">
+      <c r="O20" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R20" s="1" t="s">
@@ -2246,7 +2228,7 @@
       <c r="A21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2285,13 +2267,13 @@
       <c r="N21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O21" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q21" s="5" t="s">
+      <c r="O21" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R21" s="1" t="s">
@@ -2314,7 +2296,7 @@
       <c r="A22" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -2353,13 +2335,13 @@
       <c r="N22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O22" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q22" s="5" t="s">
+      <c r="O22" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R22" s="1" t="s">
@@ -2382,7 +2364,7 @@
       <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -2421,13 +2403,13 @@
       <c r="N23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O23" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q23" s="5" t="s">
+      <c r="O23" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R23" s="1" t="s">
@@ -2450,7 +2432,7 @@
       <c r="A24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2487,28 +2469,28 @@
       <c r="N24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O24" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q24" s="5" t="s">
+      <c r="O24" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R24" t="s">
         <v>29</v>
       </c>
-      <c r="S24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U24" s="6">
+      <c r="S24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U24" s="5">
         <v>300</v>
       </c>
-      <c r="V24" s="7" t="s">
+      <c r="V24" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2516,7 +2498,7 @@
       <c r="A25" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2555,13 +2537,13 @@
       <c r="N25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O25" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q25" s="5" t="s">
+      <c r="O25" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R25" s="1" t="s">
@@ -2584,7 +2566,7 @@
       <c r="A26" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -2623,13 +2605,13 @@
       <c r="N26" t="s">
         <v>29</v>
       </c>
-      <c r="O26" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q26" s="5" t="s">
+      <c r="O26" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R26" s="1" t="s">
@@ -2652,7 +2634,7 @@
       <c r="A27" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -2691,13 +2673,13 @@
       <c r="N27" t="s">
         <v>29</v>
       </c>
-      <c r="O27" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q27" s="5" t="s">
+      <c r="O27" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -2720,7 +2702,7 @@
       <c r="A28" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -2759,13 +2741,13 @@
       <c r="N28" t="s">
         <v>29</v>
       </c>
-      <c r="O28" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q28" s="5" t="s">
+      <c r="O28" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -2788,7 +2770,7 @@
       <c r="A29" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2827,28 +2809,28 @@
       <c r="N29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O29" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q29" s="5" t="s">
+      <c r="O29" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S29" s="6">
+      <c r="S29" s="5">
         <v>100</v>
       </c>
-      <c r="T29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="V29" s="7" t="s">
+      <c r="T29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V29" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2856,7 +2838,7 @@
       <c r="A30" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2895,28 +2877,28 @@
       <c r="N30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O30" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q30" s="5" t="s">
+      <c r="O30" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S30" s="6">
+      <c r="S30" s="5">
         <v>50</v>
       </c>
-      <c r="T30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="V30" s="7" t="s">
+      <c r="T30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V30" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2924,7 +2906,7 @@
       <c r="A31" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2963,28 +2945,28 @@
       <c r="N31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O31" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="5" t="s">
+      <c r="O31" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T31" s="6">
+      <c r="S31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T31" s="5">
         <v>300</v>
       </c>
-      <c r="U31" s="6">
+      <c r="U31" s="5">
         <v>300</v>
       </c>
-      <c r="V31" s="7" t="s">
+      <c r="V31" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2992,7 +2974,7 @@
       <c r="A32" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -3031,28 +3013,28 @@
       <c r="N32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q32" s="5" t="s">
+      <c r="O32" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U32" s="6">
+      <c r="S32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U32" s="5">
         <v>300</v>
       </c>
-      <c r="V32" s="7" t="s">
+      <c r="V32" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3060,7 +3042,7 @@
       <c r="A33" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -3099,28 +3081,28 @@
       <c r="N33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O33" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q33" s="5" t="s">
+      <c r="O33" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U33" s="6">
+      <c r="S33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U33" s="5">
         <v>300</v>
       </c>
-      <c r="V33" s="7" t="s">
+      <c r="V33" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3128,7 +3110,7 @@
       <c r="A34" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -3167,13 +3149,13 @@
       <c r="N34" t="s">
         <v>29</v>
       </c>
-      <c r="O34" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q34" s="5" t="s">
+      <c r="O34" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R34" s="1" t="s">
@@ -3196,7 +3178,7 @@
       <c r="A35" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -3235,13 +3217,13 @@
       <c r="N35" t="s">
         <v>29</v>
       </c>
-      <c r="O35" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q35" s="5" t="s">
+      <c r="O35" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q35" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R35" s="1" t="s">
@@ -3264,7 +3246,7 @@
       <c r="A36" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -3303,25 +3285,25 @@
       <c r="N36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O36" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R36" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S36" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T36" s="6">
+      <c r="O36" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" s="5">
         <v>300</v>
       </c>
-      <c r="U36" s="7" t="s">
+      <c r="U36" s="6" t="s">
         <v>29</v>
       </c>
       <c r="V36" t="s">
@@ -3332,7 +3314,7 @@
       <c r="A37" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -3371,13 +3353,13 @@
       <c r="N37" t="s">
         <v>29</v>
       </c>
-      <c r="O37" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q37" s="5" t="s">
+      <c r="O37" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R37" s="1">
@@ -3400,7 +3382,7 @@
       <c r="A38" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -3439,28 +3421,28 @@
       <c r="N38" t="s">
         <v>29</v>
       </c>
-      <c r="O38" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P38" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q38" s="5" t="s">
+      <c r="O38" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q38" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T38" s="6">
+      <c r="S38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T38" s="5">
         <v>300</v>
       </c>
-      <c r="U38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="V38" s="7" t="s">
+      <c r="U38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V38" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3468,7 +3450,7 @@
       <c r="A39" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -3507,13 +3489,13 @@
       <c r="N39" t="s">
         <v>49</v>
       </c>
-      <c r="O39" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q39" s="5" t="s">
+      <c r="O39" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R39" s="1" t="s">
@@ -3536,7 +3518,7 @@
       <c r="A40" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -3575,13 +3557,13 @@
       <c r="N40" t="s">
         <v>49</v>
       </c>
-      <c r="O40" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P40" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q40" s="5" t="s">
+      <c r="O40" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -3604,7 +3586,7 @@
       <c r="A41" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -3643,13 +3625,13 @@
       <c r="N41" t="s">
         <v>49</v>
       </c>
-      <c r="O41" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P41" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q41" s="5" t="s">
+      <c r="O41" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R41" s="1" t="s">
@@ -3672,7 +3654,7 @@
       <c r="A42" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -3711,13 +3693,13 @@
       <c r="N42" t="s">
         <v>49</v>
       </c>
-      <c r="O42" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q42" s="5" t="s">
+      <c r="O42" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R42" s="1" t="s">
@@ -3740,7 +3722,7 @@
       <c r="A43" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -3779,13 +3761,13 @@
       <c r="N43" t="s">
         <v>129</v>
       </c>
-      <c r="O43" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P43" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q43" s="5" t="s">
+      <c r="O43" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R43" s="1" t="s">
@@ -3808,7 +3790,7 @@
       <c r="A44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -3847,13 +3829,13 @@
       <c r="N44" t="s">
         <v>49</v>
       </c>
-      <c r="O44" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q44" s="5" t="s">
+      <c r="O44" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R44">
@@ -3876,7 +3858,7 @@
       <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3915,13 +3897,13 @@
       <c r="N45" t="s">
         <v>49</v>
       </c>
-      <c r="O45" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q45" s="5" t="s">
+      <c r="O45" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R45">
@@ -3944,7 +3926,7 @@
       <c r="A46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -3983,13 +3965,13 @@
       <c r="N46" t="s">
         <v>49</v>
       </c>
-      <c r="O46" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q46" s="5" t="s">
+      <c r="O46" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q46" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R46">
@@ -4012,7 +3994,7 @@
       <c r="A47" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -4051,13 +4033,13 @@
       <c r="N47" t="s">
         <v>49</v>
       </c>
-      <c r="O47" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q47" s="5" t="s">
+      <c r="O47" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q47" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R47">
@@ -4080,7 +4062,7 @@
       <c r="A48" t="s">
         <v>137</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -4119,13 +4101,13 @@
       <c r="N48" t="s">
         <v>139</v>
       </c>
-      <c r="O48" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P48" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q48" s="5" t="s">
+      <c r="O48" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q48" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R48">
@@ -4148,7 +4130,7 @@
       <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -4187,13 +4169,13 @@
       <c r="N49" t="s">
         <v>29</v>
       </c>
-      <c r="O49" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P49" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q49" s="5" t="s">
+      <c r="O49" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q49" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R49">
@@ -4216,7 +4198,7 @@
       <c r="A50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -4255,13 +4237,13 @@
       <c r="N50" t="s">
         <v>29</v>
       </c>
-      <c r="O50" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q50" s="5" t="s">
+      <c r="O50" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R50">
@@ -4284,7 +4266,7 @@
       <c r="A51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -4323,13 +4305,13 @@
       <c r="N51" t="s">
         <v>29</v>
       </c>
-      <c r="O51" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q51" s="5" t="s">
+      <c r="O51" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R51">
@@ -4352,7 +4334,7 @@
       <c r="A52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -4391,13 +4373,13 @@
       <c r="N52" t="s">
         <v>29</v>
       </c>
-      <c r="O52" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q52" s="5" t="s">
+      <c r="O52" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q52" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R52" t="s">
@@ -4420,7 +4402,7 @@
       <c r="A53" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -4459,13 +4441,13 @@
       <c r="N53" t="s">
         <v>29</v>
       </c>
-      <c r="O53" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P53" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q53" s="5" t="s">
+      <c r="O53" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P53" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q53" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R53" t="s">
@@ -4488,7 +4470,7 @@
       <c r="A54" t="s">
         <v>150</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -4527,13 +4509,13 @@
       <c r="N54" t="s">
         <v>49</v>
       </c>
-      <c r="O54" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P54" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q54" s="5" t="s">
+      <c r="O54" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P54" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q54" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R54" t="s">
@@ -4556,7 +4538,7 @@
       <c r="A55" t="s">
         <v>153</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -4595,13 +4577,13 @@
       <c r="N55" t="s">
         <v>49</v>
       </c>
-      <c r="O55" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P55" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q55" s="5" t="s">
+      <c r="O55" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P55" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q55" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R55" t="s">
@@ -4624,7 +4606,7 @@
       <c r="A56" t="s">
         <v>155</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -4663,13 +4645,13 @@
       <c r="N56" t="s">
         <v>49</v>
       </c>
-      <c r="O56" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P56" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q56" s="5" t="s">
+      <c r="O56" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q56" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R56" t="s">
@@ -4692,7 +4674,7 @@
       <c r="A57" t="s">
         <v>157</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -4731,13 +4713,13 @@
       <c r="N57" t="s">
         <v>49</v>
       </c>
-      <c r="O57" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P57" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q57" s="5" t="s">
+      <c r="O57" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P57" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q57" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R57" t="s">
@@ -4760,7 +4742,7 @@
       <c r="A58" t="s">
         <v>159</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -4799,13 +4781,13 @@
       <c r="N58" t="s">
         <v>49</v>
       </c>
-      <c r="O58" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P58" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q58" s="5" t="s">
+      <c r="O58" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P58" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q58" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R58" t="s">
@@ -4828,7 +4810,7 @@
       <c r="A59" t="s">
         <v>161</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -4867,13 +4849,13 @@
       <c r="N59" t="s">
         <v>49</v>
       </c>
-      <c r="O59" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P59" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q59" s="5" t="s">
+      <c r="O59" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P59" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q59" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R59">
@@ -4896,7 +4878,7 @@
       <c r="A60" t="s">
         <v>163</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -4935,13 +4917,13 @@
       <c r="N60" t="s">
         <v>49</v>
       </c>
-      <c r="O60" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P60" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q60" s="5" t="s">
+      <c r="O60" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P60" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q60" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R60">
@@ -4964,7 +4946,7 @@
       <c r="A61" t="s">
         <v>165</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -5003,13 +4985,13 @@
       <c r="N61" t="s">
         <v>49</v>
       </c>
-      <c r="O61" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P61" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q61" s="5" t="s">
+      <c r="O61" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q61" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R61">
@@ -5032,7 +5014,7 @@
       <c r="A62" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -5071,13 +5053,13 @@
       <c r="N62" t="s">
         <v>49</v>
       </c>
-      <c r="O62" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P62" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q62" s="5" t="s">
+      <c r="O62" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P62" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q62" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R62">
@@ -5100,7 +5082,7 @@
       <c r="A63" t="s">
         <v>169</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -5139,13 +5121,13 @@
       <c r="N63" t="s">
         <v>49</v>
       </c>
-      <c r="O63" s="5">
-        <v>45384</v>
-      </c>
-      <c r="P63" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q63" s="5" t="s">
+      <c r="O63" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q63" s="4" t="s">
         <v>31</v>
       </c>
       <c r="R63">

</xml_diff>